<commit_message>
improving toc with array formulas
</commit_message>
<xml_diff>
--- a/examples/sbtab-sbml/ecoli_noor_2016_data.xlsx
+++ b/examples/sbtab-sbml/ecoli_noor_2016_data.xlsx
@@ -6422,7 +6422,7 @@
     <t>'!rxnconReactionList'!A1</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='TableOfContents' Description='Table of contents' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='TableOfContents' Description='Table of contents' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Table</t>
@@ -6512,7 +6512,7 @@
     <t>rxnconReactionList</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Compartment' ModelName='Compartment' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Compartment' ModelName='Compartment' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Comment</t>
@@ -6572,7 +6572,7 @@
     <t>!Identifiers:sbo.go</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Compound' ModelName='Compound' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Compound' ModelName='Compound' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!SBML:species:id</t>
@@ -6635,7 +6635,7 @@
     <t>!NameForPlots</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Definition' ModelName='Definition' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Definition' ModelName='Definition' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!ComponentName</t>
@@ -6650,7 +6650,7 @@
     <t>!Format</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Enzyme' ModelName='Enzyme' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Enzyme' ModelName='Enzyme' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!CatalysedReaction</t>
@@ -6671,7 +6671,7 @@
     <t>!Gene</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='FbcObjective' ModelName='FbcObjective' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='FbcObjective' ModelName='FbcObjective' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!SBML:fbc:type</t>
@@ -6686,7 +6686,7 @@
     <t>!SBML:fbc:reaction</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Gene' ModelName='Gene' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Gene' ModelName='Gene' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!LocusName</t>
@@ -6716,7 +6716,7 @@
     <t>!SBML:fbc:Label</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Layout' ModelName='Layout' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Layout' ModelName='Layout' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!SBML:layout:modelEntity</t>
@@ -6752,7 +6752,7 @@
     <t>!SBML:layout:speciesRole</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Measurement' ModelName='Measurement' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Measurement' ModelName='Measurement' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Sample</t>
@@ -6764,7 +6764,7 @@
     <t>!ValueType</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='PbConfig' ModelName='PbConfig' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='PbConfig' ModelName='PbConfig' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Option</t>
@@ -6773,16 +6773,16 @@
     <t>!Value</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Position' ModelName='Position' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Position' ModelName='Position' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Element</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Protein' ModelName='Protein' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
-  </si>
-  <si>
-    <t>!!ObjTables TableType='Data' ModelId='Quantity' ModelName='Quantity' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8' Document='E. coli central carbon metabolism - unbalanced kinetic data'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Protein' ModelName='Protein' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8'</t>
+  </si>
+  <si>
+    <t>!!ObjTables TableType='Data' ModelId='Quantity' ModelName='Quantity' Date='2019-09-23 12:47:18' ObjTablesVersion='0.0.8' Document='E. coli central carbon metabolism - unbalanced kinetic data'</t>
   </si>
   <si>
     <t>!Quantity</t>
@@ -7385,7 +7385,7 @@
     <t>product catalytic rate constant</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='QuantityInfo' ModelName='QuantityInfo' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='QuantityInfo' ModelName='QuantityInfo' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Constant</t>
@@ -7403,7 +7403,7 @@
     <t>!SBMLElementType</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='QuantityMatrix' ModelName='QuantityMatrix' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='QuantityMatrix' ModelName='QuantityMatrix' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!&gt;Table:Column</t>
@@ -7442,7 +7442,7 @@
     <t>!&gt;TP:t1:std</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Reaction' ModelName='Reaction' Date='2019-09-23 11:04:40' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Reaction' ModelName='Reaction' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Modifier</t>
@@ -7514,7 +7514,7 @@
     <t>!Regulator</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='ReactionStoichiometry' ModelName='ReactionStoichiometry' Date='2019-09-23 11:04:41' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='ReactionStoichiometry' ModelName='ReactionStoichiometry' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Stoichiometry</t>
@@ -7526,7 +7526,7 @@
     <t>!Product</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Regulator' ModelName='Regulator' Date='2019-09-23 11:04:41' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Regulator' ModelName='Regulator' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!TargetGene</t>
@@ -7538,7 +7538,7 @@
     <t>!TargetPromoter</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Relation' ModelName='Relation' Date='2019-09-23 11:04:41' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Relation' ModelName='Relation' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!From</t>
@@ -7553,13 +7553,13 @@
     <t>!Value:QuantityType</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='Relationship' ModelName='Relationship' Date='2019-09-23 11:04:41' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='Relationship' ModelName='Relationship' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!Relation</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='SparseMatrix' ModelName='SparseMatrix' Date='2019-09-23 11:04:41' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='SparseMatrix' ModelName='SparseMatrix' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!RowID</t>
@@ -7568,13 +7568,13 @@
     <t>!ColumnID</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='SparseMatrixColumn' ModelName='SparseMatrixColumn' Date='2019-09-23 11:04:41' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='SparseMatrixColumn' ModelName='SparseMatrixColumn' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!ColumnString</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='SparseMatrixOrdered' ModelName='SparseMatrixOrdered' Date='2019-09-23 11:04:41' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='SparseMatrixOrdered' ModelName='SparseMatrixOrdered' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!RowNumber</t>
@@ -7583,19 +7583,19 @@
     <t>!ColumnNumber</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='SparseMatrixRow' ModelName='SparseMatrixRow' Date='2019-09-23 11:04:41' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='SparseMatrixRow' ModelName='SparseMatrixRow' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!RowString</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='StoichiometricMatrix' ModelName='StoichiometricMatrix' Date='2019-09-23 11:04:41' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='StoichiometricMatrix' ModelName='StoichiometricMatrix' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!ReactionID</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='rxnconContingencyList' ModelName='rxnconContingencyList' Date='2019-09-23 11:04:41' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='rxnconContingencyList' ModelName='rxnconContingencyList' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!UID:Contingency</t>
@@ -7616,7 +7616,7 @@
     <t>!InternalComplexID</t>
   </si>
   <si>
-    <t>!!ObjTables TableType='Data' ModelId='rxnconReactionList' ModelName='rxnconReactionList' Date='2019-09-23 11:04:41' ObjTablesVersion='0.0.8'</t>
+    <t>!!ObjTables TableType='Data' ModelId='rxnconReactionList' ModelName='rxnconReactionList' Date='2019-09-23 12:47:19' ObjTablesVersion='0.0.8'</t>
   </si>
   <si>
     <t>!UID:Reaction</t>
@@ -8051,7 +8051,7 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
-        <f>COUNTA('!Compartment'!A3:A1048576)</f>
+        <f t="array" ref="C3">SUM((COUNTBLANK(OFFSET('!Compartment'!A3, ROW(1:1048574)-1, 0, 1, 20))&lt;&gt;20)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8061,7 +8061,7 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4">
-        <f>COUNTA('!Compound'!A3:A1048576)</f>
+        <f t="array" ref="C4">SUM((COUNTBLANK(OFFSET('!Compound'!A3, ROW(1:1048574)-1, 0, 1, 35))&lt;&gt;35)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8071,7 +8071,7 @@
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4">
-        <f>COUNTA('!Definition'!A3:A1048576)</f>
+        <f t="array" ref="C5">SUM((COUNTBLANK(OFFSET('!Definition'!A3, ROW(1:1048574)-1, 0, 1, 5))&lt;&gt;5)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8081,7 +8081,7 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4">
-        <f>COUNTA('!Enzyme'!A3:A1048576)</f>
+        <f t="array" ref="C6">SUM((COUNTBLANK(OFFSET('!Enzyme'!A3, ROW(1:1048574)-1, 0, 1, 19))&lt;&gt;19)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8091,7 +8091,7 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4">
-        <f>COUNTA('!FbcObjective'!A3:A1048576)</f>
+        <f t="array" ref="C7">SUM((COUNTBLANK(OFFSET('!FbcObjective'!A3, ROW(1:1048574)-1, 0, 1, 6))&lt;&gt;6)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8101,7 +8101,7 @@
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4">
-        <f>COUNTA('!Gene'!A3:A1048576)</f>
+        <f t="array" ref="C8">SUM((COUNTBLANK(OFFSET('!Gene'!A3, ROW(1:1048574)-1, 0, 1, 22))&lt;&gt;22)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8111,7 +8111,7 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4">
-        <f>COUNTA('!Layout'!A3:A1048576)</f>
+        <f t="array" ref="C9">SUM((COUNTBLANK(OFFSET('!Layout'!A3, ROW(1:1048574)-1, 0, 1, 13))&lt;&gt;13)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8121,7 +8121,7 @@
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4">
-        <f>COUNTA('!Measurement'!A3:A1048576)</f>
+        <f t="array" ref="C10">SUM((COUNTBLANK(OFFSET('!Measurement'!A3, ROW(1:1048574)-1, 0, 1, 5))&lt;&gt;5)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8131,7 +8131,7 @@
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4">
-        <f>COUNTA('!PbConfig'!A3:A1048576)</f>
+        <f t="array" ref="C11">SUM((COUNTBLANK(OFFSET('!PbConfig'!A3, ROW(1:1048574)-1, 0, 1, 2))&lt;&gt;2)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8141,7 +8141,7 @@
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
-        <f>COUNTA('!Position'!A3:A1048576)</f>
+        <f t="array" ref="C12">SUM((COUNTBLANK(OFFSET('!Position'!A3, ROW(1:1048574)-1, 0, 1, 3))&lt;&gt;3)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8151,7 +8151,7 @@
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
-        <f>COUNTA('!Protein'!A3:A1048576)</f>
+        <f t="array" ref="C13">SUM((COUNTBLANK(OFFSET('!Protein'!A3, ROW(1:1048574)-1, 0, 1, 15))&lt;&gt;15)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8161,7 +8161,7 @@
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4">
-        <f>COUNTA('!Quantity'!A3:A1048576)</f>
+        <f t="array" ref="C14">SUM((COUNTBLANK(OFFSET('!Quantity'!A3, ROW(1:1048574)-1, 0, 1, 75))&lt;&gt;75)*1)</f>
         <v>227</v>
       </c>
     </row>
@@ -8171,7 +8171,7 @@
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4">
-        <f>COUNTA('!QuantityInfo'!A3:A1048576)</f>
+        <f t="array" ref="C15">SUM((COUNTBLANK(OFFSET('!QuantityInfo'!A3, ROW(1:1048574)-1, 0, 1, 19))&lt;&gt;19)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
-        <f>COUNTA('!QuantityMatrix'!A3:A1048576)</f>
+        <f t="array" ref="C16">SUM((COUNTBLANK(OFFSET('!QuantityMatrix'!A3, ROW(1:1048574)-1, 0, 1, 49))&lt;&gt;49)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8191,7 +8191,7 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4">
-        <f>COUNTA('!Reaction'!A3:A1048576)</f>
+        <f t="array" ref="C17">SUM((COUNTBLANK(OFFSET('!Reaction'!A3, ROW(1:1048574)-1, 0, 1, 47))&lt;&gt;47)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8201,7 +8201,7 @@
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4">
-        <f>COUNTA('!ReactionStoichiometry'!A3:A1048576)</f>
+        <f t="array" ref="C18">SUM((COUNTBLANK(OFFSET('!ReactionStoichiometry'!A3, ROW(1:1048574)-1, 0, 1, 6))&lt;&gt;6)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8211,7 +8211,7 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4">
-        <f>COUNTA('!Regulator'!A3:A1048576)</f>
+        <f t="array" ref="C19">SUM((COUNTBLANK(OFFSET('!Regulator'!A3, ROW(1:1048574)-1, 0, 1, 17))&lt;&gt;17)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8221,7 +8221,7 @@
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4">
-        <f>COUNTA('!Relation'!A3:A1048576)</f>
+        <f t="array" ref="C20">SUM((COUNTBLANK(OFFSET('!Relation'!A3, ROW(1:1048574)-1, 0, 1, 10))&lt;&gt;10)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8231,7 +8231,7 @@
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4">
-        <f>COUNTA('!Relationship'!A3:A1048576)</f>
+        <f t="array" ref="C21">SUM((COUNTBLANK(OFFSET('!Relationship'!A3, ROW(1:1048574)-1, 0, 1, 7))&lt;&gt;7)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8241,7 +8241,7 @@
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4">
-        <f>COUNTA('!SparseMatrix'!A3:A1048576)</f>
+        <f t="array" ref="C22">SUM((COUNTBLANK(OFFSET('!SparseMatrix'!A3, ROW(1:1048574)-1, 0, 1, 3))&lt;&gt;3)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8251,7 +8251,7 @@
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4">
-        <f>COUNTA('!SparseMatrixColumn'!A3:A1048576)</f>
+        <f t="array" ref="C23">SUM((COUNTBLANK(OFFSET('!SparseMatrixColumn'!A3, ROW(1:1048574)-1, 0, 1, 2))&lt;&gt;2)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8261,7 +8261,7 @@
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4">
-        <f>COUNTA('!SparseMatrixOrdered'!A3:A1048576)</f>
+        <f t="array" ref="C24">SUM((COUNTBLANK(OFFSET('!SparseMatrixOrdered'!A3, ROW(1:1048574)-1, 0, 1, 3))&lt;&gt;3)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8271,7 +8271,7 @@
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4">
-        <f>COUNTA('!SparseMatrixRow'!A3:A1048576)</f>
+        <f t="array" ref="C25">SUM((COUNTBLANK(OFFSET('!SparseMatrixRow'!A3, ROW(1:1048574)-1, 0, 1, 2))&lt;&gt;2)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8281,7 +8281,7 @@
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4">
-        <f>COUNTA('!StoichiometricMatrix'!A3:A1048576)</f>
+        <f t="array" ref="C26">SUM((COUNTBLANK(OFFSET('!StoichiometricMatrix'!A3, ROW(1:1048574)-1, 0, 1, 5))&lt;&gt;5)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8291,7 +8291,7 @@
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4">
-        <f>COUNTA('!rxnconContingencyList'!A3:A1048576)</f>
+        <f t="array" ref="C27">SUM((COUNTBLANK(OFFSET('!rxnconContingencyList'!A3, ROW(1:1048574)-1, 0, 1, 8))&lt;&gt;8)*1)</f>
         <v>0</v>
       </c>
     </row>
@@ -8301,7 +8301,7 @@
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4">
-        <f>COUNTA('!rxnconReactionList'!A3:A1048576)</f>
+        <f t="array" ref="C28">SUM((COUNTBLANK(OFFSET('!rxnconReactionList'!A3, ROW(1:1048574)-1, 0, 1, 12))&lt;&gt;12)*1)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>